<commit_message>
Updated Sprint6 Stand up meeting Templet.
</commit_message>
<xml_diff>
--- a/Project_Files/Sprint 6/Stand-up Meeting Sprint6.xlsx
+++ b/Project_Files/Sprint 6/Stand-up Meeting Sprint6.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s546907\Downloads\GDP PROJECT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S547049\Documents\GitHub\FreebiesforNewbies\Project_Files\Sprint 6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B45D0426-E542-48D0-B3D8-C7B3C3A775FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{193FF9CE-4924-4856-BC03-7D14F2963A99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="380" windowWidth="19180" windowHeight="10180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="33">
   <si>
     <t>Monday</t>
   </si>
@@ -159,6 +159,30 @@
   </si>
   <si>
     <t>3) Over coming stage fear</t>
+  </si>
+  <si>
+    <t>1) Did changes on ER diagram</t>
+  </si>
+  <si>
+    <t>3) NA</t>
+  </si>
+  <si>
+    <t>1) Finalaized ER diagram and learned about Android studio and how to integrate Firebase Database in Android studio.</t>
+  </si>
+  <si>
+    <t>2) I will change the Database based on project requirement.</t>
+  </si>
+  <si>
+    <t>3) We are finalizing the database.</t>
+  </si>
+  <si>
+    <t>2) I will give presentaion on Firebase database and will do changes in ER diagram.</t>
+  </si>
+  <si>
+    <t>2) I will prepare workshop presentation document on Firebase databse.</t>
+  </si>
+  <si>
+    <t>1)Prepared Workshop resentation slides on Firebase database and learned queries and architecture.</t>
   </si>
 </sst>
 </file>
@@ -350,6 +374,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -358,18 +394,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -653,8 +677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -666,52 +690,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
@@ -747,7 +771,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="46.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="14"/>
+      <c r="A9" s="11"/>
       <c r="B9" s="5" t="s">
         <v>19</v>
       </c>
@@ -759,7 +783,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="15"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="5" t="s">
         <v>17</v>
       </c>
@@ -771,7 +795,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -785,7 +809,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A12" s="14"/>
+      <c r="A12" s="11"/>
       <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
@@ -797,7 +821,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A13" s="15"/>
+      <c r="A13" s="12"/>
       <c r="B13" s="3" t="s">
         <v>6</v>
       </c>
@@ -808,46 +832,46 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="62" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A15" s="14"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="46.5" x14ac:dyDescent="0.3">
+      <c r="A15" s="11"/>
       <c r="B15" s="5" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A16" s="15"/>
+      <c r="A16" s="12"/>
       <c r="B16" s="5" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="10" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -861,7 +885,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A18" s="14"/>
+      <c r="A18" s="11"/>
       <c r="B18" s="3" t="s">
         <v>5</v>
       </c>
@@ -873,7 +897,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A19" s="15"/>
+      <c r="A19" s="12"/>
       <c r="B19" s="3" t="s">
         <v>6</v>
       </c>
@@ -899,7 +923,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A21" s="14"/>
+      <c r="A21" s="11"/>
       <c r="B21" s="5" t="s">
         <v>5</v>
       </c>
@@ -911,7 +935,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A22" s="15"/>
+      <c r="A22" s="12"/>
       <c r="B22" s="5" t="s">
         <v>6</v>
       </c>
@@ -929,18 +953,18 @@
       <c r="B25" s="6"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="12"/>
+      <c r="B26" s="9"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12"/>
+      <c r="A27" s="9"/>
+      <c r="B27" s="9"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
     </row>
     <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Updated standup meeting excel
Updated the daily motives in the standup meeting file
</commit_message>
<xml_diff>
--- a/Project_Files/Sprint 6/Stand-up Meeting Sprint6.xlsx
+++ b/Project_Files/Sprint 6/Stand-up Meeting Sprint6.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S547076\Desktop\FreebiesforNewbies\Project_Files\Sprint 6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nwmissouri-my.sharepoint.com/personal/s546981_nwmissouri_edu/Documents/Documents/GitHub/FreebiesforNewbies/Project_Files/Sprint 6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E9CF444-AECF-4CD3-A7A4-FDCAAFE4F208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{3E9CF444-AECF-4CD3-A7A4-FDCAAFE4F208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0FE0FABD-ED18-4340-BE8F-61A25078D9A6}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="20" windowWidth="19180" windowHeight="10180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
   <si>
     <t>Monday</t>
   </si>
@@ -207,6 +207,27 @@
   </si>
   <si>
     <t xml:space="preserve">We are taking a step to database  </t>
+  </si>
+  <si>
+    <t>1)Learned about recycler view and components of the android</t>
+  </si>
+  <si>
+    <t>2)Preparing slides for presentation</t>
+  </si>
+  <si>
+    <t>3) Finalizing the database</t>
+  </si>
+  <si>
+    <t>1) Prepared slides for the workshop</t>
+  </si>
+  <si>
+    <t>2)I will give presentation today</t>
+  </si>
+  <si>
+    <t>1)I prepared and given presentation today</t>
+  </si>
+  <si>
+    <t>2)Discussing about pros and cons heroku progress today</t>
   </si>
 </sst>
 </file>
@@ -701,8 +722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -894,42 +915,42 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="31" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15.5" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="31" x14ac:dyDescent="0.3">
       <c r="A18" s="11"/>
       <c r="B18" s="3" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A19" s="12"/>
       <c r="B19" s="3" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="31" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
made changes to stand-up meeting
</commit_message>
<xml_diff>
--- a/Project_Files/Sprint 6/Stand-up Meeting Sprint6.xlsx
+++ b/Project_Files/Sprint 6/Stand-up Meeting Sprint6.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nwmissouri-my.sharepoint.com/personal/s546981_nwmissouri_edu/Documents/Documents/GitHub/FreebiesforNewbies/Project_Files/Sprint 6/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nwmissouri-my.sharepoint.com/personal/s546907_nwmissouri_edu/Documents/Desktop/git-local-repo/FreebiesforNewbies/Project_Files/Sprint 6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{3E9CF444-AECF-4CD3-A7A4-FDCAAFE4F208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0FE0FABD-ED18-4340-BE8F-61A25078D9A6}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{3E9CF444-AECF-4CD3-A7A4-FDCAAFE4F208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B797666D-6C25-4E90-8E36-EF418167404C}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="20" windowWidth="19180" windowHeight="10180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="53">
   <si>
     <t>Monday</t>
   </si>
@@ -40,12 +40,6 @@
   </si>
   <si>
     <t>Daily Stand-up Meeting Report</t>
-  </si>
-  <si>
-    <t>1)</t>
-  </si>
-  <si>
-    <t>2)</t>
   </si>
   <si>
     <t>3)</t>
@@ -229,12 +223,33 @@
   <si>
     <t>2)Discussing about pros and cons heroku progress today</t>
   </si>
+  <si>
+    <t>Na</t>
+  </si>
+  <si>
+    <t>1.Searched the requirements for workshop.</t>
+  </si>
+  <si>
+    <t>1.I completed the ppt my part of presentation.</t>
+  </si>
+  <si>
+    <t>2Did some background work on android studio and layouts.</t>
+  </si>
+  <si>
+    <t>2. I completed the analysis requirements of the functionality.</t>
+  </si>
+  <si>
+    <t>3.)Need to make the ppt work greatfully.</t>
+  </si>
+  <si>
+    <t>3. I need to work on the functionality no time for coding.Hectic schedule.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -287,6 +302,16 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF252525"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF252525"/>
+      <name val="&quot;Times New Roman&quot;"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -314,7 +339,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -400,11 +425,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -439,6 +479,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -722,11 +768,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="23" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.6328125" style="1" bestFit="1" customWidth="1"/>
@@ -734,7 +780,7 @@
     <col min="7" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="A1" s="14" t="s">
         <v>3</v>
       </c>
@@ -744,7 +790,7 @@
       <c r="E1" s="14"/>
       <c r="F1" s="14"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6">
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
@@ -752,9 +798,9 @@
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6">
       <c r="A3" s="15" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" s="15"/>
       <c r="C3" s="15"/>
@@ -762,9 +808,9 @@
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6">
       <c r="A4" s="15" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4" s="15"/>
       <c r="C4" s="15"/>
@@ -772,9 +818,9 @@
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6">
       <c r="A5" s="16" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" s="16"/>
       <c r="C5" s="16"/>
@@ -782,14 +828,14 @@
       <c r="E5" s="16"/>
       <c r="F5" s="16"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6">
       <c r="A7" s="2"/>
       <c r="B7" s="4" t="s">
         <v>0</v>
@@ -801,219 +847,219 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="31" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="31">
       <c r="A8" s="13" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="46.5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:6" ht="46.5">
       <c r="A9" s="11"/>
       <c r="B9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="D9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:6" ht="15.5">
       <c r="A10" s="12"/>
       <c r="B10" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15.5" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="31">
       <c r="A11" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15.5" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="31">
       <c r="A12" s="11"/>
-      <c r="B12" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="B12" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="31">
       <c r="A13" s="12"/>
-      <c r="B13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="62" x14ac:dyDescent="0.3">
+      <c r="B13" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="62">
       <c r="A14" s="13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="46.5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:6" ht="46.5">
       <c r="A15" s="11"/>
       <c r="B15" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15.5" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.5">
       <c r="A16" s="12"/>
       <c r="B16" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="31" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="31">
       <c r="A17" s="10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="31" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:4" ht="31">
       <c r="A18" s="11"/>
       <c r="B18" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C18" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="15.5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:4" ht="15.5">
       <c r="A19" s="12"/>
       <c r="B19" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="31" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="31">
       <c r="A20" s="13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="46.5" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="46.5">
       <c r="A21" s="11"/>
       <c r="B21" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>36</v>
-      </c>
       <c r="D21" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15.5" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.5">
       <c r="A22" s="12"/>
       <c r="B22" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C22" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15">
+      <c r="A25" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="6"/>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" s="6"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="8" t="s">
-        <v>8</v>
-      </c>
       <c r="B26" s="9"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4">
       <c r="A27" s="9"/>
       <c r="B27" s="9"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4">
       <c r="A28" s="9"/>
       <c r="B28" s="9"/>
     </row>
-    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="44" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="33" ht="15.75" customHeight="1"/>
+    <row r="44" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="A26:B28"/>

</xml_diff>

<commit_message>
Updated Sprint7 Team Reports and Individual Reports
updated Team report, stand-up meeting template, Midterm presentation slides, individual reports for Sprint7
</commit_message>
<xml_diff>
--- a/Project_Files/Sprint 6/Stand-up Meeting Sprint6.xlsx
+++ b/Project_Files/Sprint 6/Stand-up Meeting Sprint6.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -459,6 +459,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -479,12 +485,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -768,8 +768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14"/>
@@ -781,52 +781,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2"/>
@@ -848,7 +848,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="31">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="15" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -862,7 +862,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="46.5">
-      <c r="A9" s="11"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="5" t="s">
         <v>17</v>
       </c>
@@ -874,7 +874,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.5">
-      <c r="A10" s="12"/>
+      <c r="A10" s="14"/>
       <c r="B10" s="5" t="s">
         <v>15</v>
       </c>
@@ -886,45 +886,45 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="31">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="8" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="31">
-      <c r="A12" s="11"/>
-      <c r="B12" s="17" t="s">
+      <c r="A12" s="13"/>
+      <c r="B12" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="8" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="31">
-      <c r="A13" s="12"/>
-      <c r="B13" s="17" t="s">
+      <c r="A13" s="14"/>
+      <c r="B13" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="8" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="62">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="15" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -938,7 +938,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="46.5">
-      <c r="A15" s="11"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="5" t="s">
         <v>29</v>
       </c>
@@ -950,7 +950,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.5">
-      <c r="A16" s="12"/>
+      <c r="A16" s="14"/>
       <c r="B16" s="5" t="s">
         <v>24</v>
       </c>
@@ -962,7 +962,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="31">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -976,7 +976,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="31">
-      <c r="A18" s="11"/>
+      <c r="A18" s="13"/>
       <c r="B18" s="3" t="s">
         <v>40</v>
       </c>
@@ -988,7 +988,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.5">
-      <c r="A19" s="12"/>
+      <c r="A19" s="14"/>
       <c r="B19" s="3" t="s">
         <v>15</v>
       </c>
@@ -1000,7 +1000,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="31">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="15" t="s">
         <v>14</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -1014,7 +1014,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="46.5">
-      <c r="A21" s="11"/>
+      <c r="A21" s="13"/>
       <c r="B21" s="5" t="s">
         <v>32</v>
       </c>
@@ -1026,7 +1026,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.5">
-      <c r="A22" s="12"/>
+      <c r="A22" s="14"/>
       <c r="B22" s="5" t="s">
         <v>33</v>
       </c>
@@ -1044,18 +1044,18 @@
       <c r="B25" s="6"/>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="9"/>
+      <c r="B26" s="11"/>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="9"/>
-      <c r="B27" s="9"/>
+      <c r="A27" s="11"/>
+      <c r="B27" s="11"/>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="9"/>
-      <c r="B28" s="9"/>
+      <c r="A28" s="11"/>
+      <c r="B28" s="11"/>
     </row>
     <row r="32" spans="1:4" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>

</xml_diff>